<commit_message>
Create, insert,  para Estudante, endereco e user
</commit_message>
<xml_diff>
--- a/Documentacao/actividades.xlsx
+++ b/Documentacao/actividades.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="54">
   <si>
     <t>Paginas</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>Nota: O nao comprimento da data limite acareta um defice de 25% do valor estipulado para cada elemento</t>
+  </si>
+  <si>
+    <t>pm</t>
   </si>
 </sst>
 </file>
@@ -397,6 +400,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -424,8 +429,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,7 +877,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -927,7 +930,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -945,7 +948,7 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
@@ -961,7 +964,7 @@
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
@@ -978,7 +981,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
@@ -995,7 +998,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
@@ -1012,7 +1015,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
@@ -1026,7 +1029,7 @@
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="22" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1043,7 +1046,7 @@
       <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
@@ -1057,7 +1060,7 @@
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
@@ -1071,7 +1074,7 @@
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="4" t="s">
         <v>45</v>
       </c>
@@ -1083,7 +1086,7 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1097,7 +1100,7 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
@@ -1111,7 +1114,7 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="4" t="s">
         <v>21</v>
       </c>
@@ -1125,7 +1128,7 @@
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="8" t="s">
         <v>22</v>
       </c>
@@ -1139,7 +1142,7 @@
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="20" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -1155,7 +1158,7 @@
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="4" t="s">
         <v>31</v>
       </c>
@@ -1169,12 +1172,12 @@
       <c r="F17" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="26">
+      <c r="G17" s="17">
         <v>43595</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="4" t="s">
         <v>27</v>
       </c>
@@ -1188,7 +1191,7 @@
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="4" t="s">
         <v>26</v>
       </c>
@@ -1202,7 +1205,7 @@
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="4" t="s">
         <v>28</v>
       </c>
@@ -1216,7 +1219,7 @@
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="4" t="s">
         <v>29</v>
       </c>
@@ -1302,7 +1305,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,7 +1340,7 @@
       <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="16" t="s">
         <v>51</v>
       </c>
       <c r="J1" s="12" t="s">
@@ -1345,7 +1348,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1364,7 +1367,7 @@
       <c r="G2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="26">
+      <c r="H2" s="17">
         <v>43595</v>
       </c>
       <c r="J2" t="s">
@@ -1372,7 +1375,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
@@ -1389,7 +1392,7 @@
       <c r="G3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="26">
+      <c r="H3" s="17">
         <v>43595</v>
       </c>
       <c r="J3" t="s">
@@ -1397,7 +1400,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
@@ -1410,7 +1413,7 @@
       <c r="G4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="26">
+      <c r="H4" s="17">
         <v>43595</v>
       </c>
       <c r="J4" t="s">
@@ -1418,7 +1421,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
@@ -1429,7 +1432,7 @@
       <c r="G5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H5" s="17">
         <v>43595</v>
       </c>
       <c r="J5" t="s">
@@ -1437,7 +1440,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
@@ -1452,7 +1455,7 @@
       <c r="G6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="17">
         <v>43595</v>
       </c>
       <c r="J6" t="s">
@@ -1460,7 +1463,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
@@ -1473,12 +1476,12 @@
       <c r="G7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="17">
         <v>43595</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="24" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1497,12 +1500,12 @@
       <c r="G8" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="17">
         <v>43595</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="4" t="s">
         <v>45</v>
       </c>
@@ -1517,12 +1520,12 @@
       <c r="G9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H9" s="17">
         <v>43595</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
@@ -1539,12 +1542,12 @@
       <c r="G10" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="17">
         <v>43595</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
@@ -1561,16 +1564,18 @@
       <c r="G11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="26">
+      <c r="H11" s="17">
         <v>43595</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="D12" s="4" t="s">
         <v>30</v>
       </c>
@@ -1583,12 +1588,12 @@
       <c r="G12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="26">
+      <c r="H12" s="17">
         <v>43595</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
@@ -1601,12 +1606,12 @@
       <c r="G13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="26">
+      <c r="H13" s="17">
         <v>43595</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="8" t="s">
         <v>22</v>
       </c>
@@ -1621,12 +1626,12 @@
       <c r="G14" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="26">
+      <c r="H14" s="17">
         <v>43595</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -1645,12 +1650,12 @@
       <c r="G15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="26">
+      <c r="H15" s="17">
         <v>43595</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="4" t="s">
         <v>31</v>
       </c>
@@ -1667,12 +1672,12 @@
       <c r="G16" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="26">
+      <c r="H16" s="17">
         <v>43595</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="4" t="s">
         <v>27</v>
       </c>
@@ -1689,12 +1694,12 @@
       <c r="G17" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="26">
+      <c r="H17" s="17">
         <v>43595</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
@@ -1709,12 +1714,12 @@
       <c r="G18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H18" s="26">
+      <c r="H18" s="17">
         <v>43595</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="4" t="s">
         <v>28</v>
       </c>
@@ -1727,12 +1732,12 @@
       <c r="G19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="26">
+      <c r="H19" s="17">
         <v>43595</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="4" t="s">
         <v>29</v>
       </c>
@@ -1749,7 +1754,7 @@
       <c r="G20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H20" s="26">
+      <c r="H20" s="17">
         <v>43595</v>
       </c>
     </row>
@@ -1865,81 +1870,81 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="9" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F9" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
+      <c r="F9" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="26"/>
     </row>
     <row r="10" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="24"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="26"/>
     </row>
     <row r="11" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
     </row>
     <row r="12" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
     </row>
     <row r="13" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="24"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
organizando as views, css, js, imgs
</commit_message>
<xml_diff>
--- a/Documentacao/actividades.xlsx
+++ b/Documentacao/actividades.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="53">
   <si>
     <t>Paginas</t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>Data Limite</t>
-  </si>
-  <si>
-    <t>Nota: O nao comprimento da data limite acareta um defice de 25% do valor estipulado para cada elemento</t>
   </si>
   <si>
     <t>pm</t>
@@ -877,7 +874,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1302,10 +1299,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1573,9 +1570,7 @@
       <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
         <v>30</v>
       </c>
@@ -1618,7 +1613,9 @@
       <c r="C14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="E14" s="8" t="s">
         <v>30</v>
       </c>
@@ -1760,11 +1757,6 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>52</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
enviar mensgens de contacto
</commit_message>
<xml_diff>
--- a/Documentacao/actividades.xlsx
+++ b/Documentacao/actividades.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="56">
   <si>
     <t>Paginas</t>
   </si>
@@ -240,7 +240,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,12 +268,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -412,7 +406,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -447,7 +440,49 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="31">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -944,7 +979,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -962,7 +997,7 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
@@ -978,7 +1013,7 @@
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
@@ -995,7 +1030,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
@@ -1012,7 +1047,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
@@ -1029,7 +1064,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
@@ -1043,7 +1078,7 @@
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1060,7 +1095,7 @@
       <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
@@ -1074,7 +1109,7 @@
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
@@ -1088,7 +1123,7 @@
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="4" t="s">
         <v>45</v>
       </c>
@@ -1100,7 +1135,7 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1114,7 +1149,7 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
@@ -1128,7 +1163,7 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="4" t="s">
         <v>21</v>
       </c>
@@ -1142,7 +1177,7 @@
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="8" t="s">
         <v>22</v>
       </c>
@@ -1156,7 +1191,7 @@
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="20" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -1172,7 +1207,7 @@
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="4" t="s">
         <v>31</v>
       </c>
@@ -1186,12 +1221,12 @@
       <c r="F17" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="17">
+      <c r="G17" s="16">
         <v>43595</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="4" t="s">
         <v>27</v>
       </c>
@@ -1205,7 +1240,7 @@
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="4" t="s">
         <v>26</v>
       </c>
@@ -1219,7 +1254,7 @@
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="4" t="s">
         <v>28</v>
       </c>
@@ -1233,7 +1268,7 @@
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="4" t="s">
         <v>29</v>
       </c>
@@ -1281,31 +1316,31 @@
     <mergeCell ref="A8:A15"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="cellIs" dxfId="24" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
       <formula>"EP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="6" operator="equal">
       <formula>"U"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:F21">
-    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="pm">
+    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="pm">
       <formula>NOT(ISERROR(SEARCH("pm",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="2" operator="containsText" text="u">
+    <cfRule type="containsText" dxfId="26" priority="2" operator="containsText" text="u">
       <formula>NOT(ISERROR(SEARCH("u",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="f">
+    <cfRule type="containsText" dxfId="25" priority="3" operator="containsText" text="f">
       <formula>NOT(ISERROR(SEARCH("f",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="4" operator="containsText" text="ep">
+    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="ep">
       <formula>NOT(ISERROR(SEARCH("ep",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1318,8 +1353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,7 +1389,7 @@
       <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>51</v>
       </c>
       <c r="J1" s="12" t="s">
@@ -1362,7 +1397,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1381,7 +1416,7 @@
       <c r="G2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="17">
+      <c r="H2" s="16">
         <v>43595</v>
       </c>
       <c r="J2" t="s">
@@ -1389,7 +1424,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
@@ -1406,7 +1441,7 @@
       <c r="G3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="16">
         <v>43595</v>
       </c>
       <c r="J3" t="s">
@@ -1414,7 +1449,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
@@ -1427,7 +1462,7 @@
       <c r="G4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="16">
         <v>43595</v>
       </c>
       <c r="J4" t="s">
@@ -1435,7 +1470,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
@@ -1446,7 +1481,7 @@
       <c r="G5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="16">
         <v>43595</v>
       </c>
       <c r="J5" t="s">
@@ -1454,7 +1489,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
@@ -1469,7 +1504,7 @@
       <c r="G6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="16">
         <v>43595</v>
       </c>
       <c r="J6" t="s">
@@ -1477,7 +1512,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
@@ -1490,12 +1525,12 @@
       <c r="G7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="16">
         <v>43595</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1511,39 +1546,45 @@
       <c r="F8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="H8" s="17">
+      <c r="G8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="16">
         <v>43595</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="4"/>
+      <c r="C9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="G9" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H9" s="17">
+        <v>46</v>
+      </c>
+      <c r="H9" s="16">
         <v>43595</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="D10" s="6" t="s">
         <v>30</v>
       </c>
@@ -1553,15 +1594,15 @@
       <c r="F10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="17">
+      <c r="G10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="16">
         <v>43595</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
@@ -1580,12 +1621,12 @@
       <c r="G11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="17">
+      <c r="H11" s="16">
         <v>43595</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
@@ -1604,12 +1645,12 @@
       <c r="G12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="16">
         <v>43595</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
@@ -1628,12 +1669,12 @@
       <c r="G13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="17">
+      <c r="H13" s="16">
         <v>43595</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="8" t="s">
         <v>22</v>
       </c>
@@ -1652,12 +1693,12 @@
       <c r="G14" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H14" s="16">
         <v>43595</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -1676,12 +1717,12 @@
       <c r="G15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15" s="16">
         <v>43595</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="4" t="s">
         <v>31</v>
       </c>
@@ -1698,12 +1739,12 @@
       <c r="G16" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="17">
+      <c r="H16" s="16">
         <v>43595</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="4" t="s">
         <v>27</v>
       </c>
@@ -1722,12 +1763,12 @@
       <c r="G17" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="17">
+      <c r="H17" s="16">
         <v>43595</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
@@ -1744,12 +1785,12 @@
       <c r="G18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H18" s="17">
+      <c r="H18" s="16">
         <v>43595</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="4" t="s">
         <v>28</v>
       </c>
@@ -1762,12 +1803,12 @@
       <c r="G19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="17">
+      <c r="H19" s="16">
         <v>43595</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="4" t="s">
         <v>29</v>
       </c>
@@ -1784,7 +1825,7 @@
       <c r="G20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H20" s="17">
+      <c r="H20" s="16">
         <v>43595</v>
       </c>
     </row>
@@ -1792,10 +1833,10 @@
       <c r="A21" s="14"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="18"/>
+      <c r="B23" s="17"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1814,84 +1855,84 @@
     <mergeCell ref="A15:A20"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="cellIs" dxfId="17" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="47" operator="equal">
       <formula>"EP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="cellIs" dxfId="16" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="46" operator="equal">
       <formula>"U"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="cellIs" dxfId="15" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="45" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:F8 C10:F20">
-    <cfRule type="containsText" dxfId="14" priority="41" operator="containsText" text="pm">
+  <conditionalFormatting sqref="C2:F20">
+    <cfRule type="containsText" dxfId="20" priority="41" operator="containsText" text="pm">
       <formula>NOT(ISERROR(SEARCH("pm",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="42" operator="containsText" text="u">
+    <cfRule type="containsText" dxfId="19" priority="42" operator="containsText" text="u">
       <formula>NOT(ISERROR(SEARCH("u",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="43" operator="containsText" text="f">
+    <cfRule type="containsText" dxfId="18" priority="43" operator="containsText" text="f">
       <formula>NOT(ISERROR(SEARCH("f",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="44" operator="containsText" text="ep">
+    <cfRule type="containsText" dxfId="17" priority="44" operator="containsText" text="ep">
       <formula>NOT(ISERROR(SEARCH("ep",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="cellIs" dxfId="10" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="40" operator="equal">
       <formula>"EP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="cellIs" dxfId="9" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="39" operator="equal">
       <formula>"U"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="cellIs" dxfId="8" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="38" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="7" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="33" operator="equal">
       <formula>"EP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="6" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="32" operator="equal">
       <formula>"U"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="5" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="31" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="4" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="26" operator="equal">
       <formula>"EP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="3" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="25" operator="equal">
       <formula>"U"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="2" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="24" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:F8 C10:F20">
-    <cfRule type="containsText" dxfId="1" priority="11" operator="containsText" text="nt">
+  <conditionalFormatting sqref="C2:F20">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="nt">
       <formula>NOT(ISERROR(SEARCH("nt",C2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
       <formula>"nt"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1911,81 +1952,81 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="9" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F9" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
+      <c r="F9" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="26"/>
     </row>
     <row r="10" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="27"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="26"/>
     </row>
     <row r="11" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
     </row>
     <row r="12" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="27"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
     </row>
     <row r="13" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
links no user, usuario pardao no admin, QoS
</commit_message>
<xml_diff>
--- a/Documentacao/actividades.xlsx
+++ b/Documentacao/actividades.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16992" windowHeight="7750" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="front-end" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="56">
   <si>
     <t>Paginas</t>
   </si>
@@ -440,49 +440,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF002060"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="25">
     <dxf>
       <fill>
         <patternFill>
@@ -926,7 +884,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -940,19 +898,19 @@
       <selection activeCell="A8" sqref="A8:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="64.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18.850000000000001" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -978,7 +936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -996,7 +954,7 @@
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
       <c r="B3" s="4" t="s">
         <v>14</v>
@@ -1012,7 +970,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="B4" s="4" t="s">
         <v>20</v>
@@ -1029,7 +987,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="18"/>
       <c r="B5" s="4" t="s">
         <v>23</v>
@@ -1046,7 +1004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" s="4" t="s">
         <v>12</v>
@@ -1063,7 +1021,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19"/>
       <c r="B7" s="8" t="s">
         <v>13</v>
@@ -1077,7 +1035,7 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>16</v>
       </c>
@@ -1094,7 +1052,7 @@
       <c r="F8" s="10"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="20"/>
       <c r="B9" s="4" t="s">
         <v>11</v>
@@ -1108,7 +1066,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="20"/>
       <c r="B10" s="4" t="s">
         <v>17</v>
@@ -1122,7 +1080,7 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="20"/>
       <c r="B11" s="4" t="s">
         <v>45</v>
@@ -1134,7 +1092,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
       <c r="B12" s="4" t="s">
         <v>18</v>
@@ -1148,7 +1106,7 @@
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
       <c r="B13" s="4" t="s">
         <v>19</v>
@@ -1162,7 +1120,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="20"/>
       <c r="B14" s="4" t="s">
         <v>21</v>
@@ -1176,7 +1134,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="23"/>
       <c r="B15" s="8" t="s">
         <v>22</v>
@@ -1190,7 +1148,7 @@
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>24</v>
       </c>
@@ -1206,7 +1164,7 @@
       </c>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="20"/>
       <c r="B17" s="4" t="s">
         <v>31</v>
@@ -1225,7 +1183,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="20"/>
       <c r="B18" s="4" t="s">
         <v>27</v>
@@ -1239,7 +1197,7 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="20"/>
       <c r="B19" s="4" t="s">
         <v>26</v>
@@ -1253,7 +1211,7 @@
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="20"/>
       <c r="B20" s="4" t="s">
         <v>28</v>
@@ -1267,7 +1225,7 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="21"/>
       <c r="B21" s="4" t="s">
         <v>29</v>
@@ -1279,32 +1237,32 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="18.350000000000001" x14ac:dyDescent="0.35">
       <c r="B24" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>41</v>
       </c>
@@ -1316,31 +1274,31 @@
     <mergeCell ref="A8:A15"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="7" operator="equal">
       <formula>"EP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="cellIs" dxfId="29" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
       <formula>"U"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:F21">
-    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="pm">
+    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="pm">
       <formula>NOT(ISERROR(SEARCH("pm",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="2" operator="containsText" text="u">
+    <cfRule type="containsText" dxfId="20" priority="2" operator="containsText" text="u">
       <formula>NOT(ISERROR(SEARCH("u",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="3" operator="containsText" text="f">
+    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="f">
       <formula>NOT(ISERROR(SEARCH("f",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="ep">
+    <cfRule type="containsText" dxfId="18" priority="4" operator="containsText" text="ep">
       <formula>NOT(ISERROR(SEARCH("ep",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1354,20 +1312,20 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18.850000000000001" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1396,7 +1354,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
@@ -1423,7 +1381,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
       <c r="B3" s="4" t="s">
         <v>14</v>
@@ -1448,7 +1406,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="B4" s="4" t="s">
         <v>20</v>
@@ -1469,7 +1427,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="18"/>
       <c r="B5" s="4" t="s">
         <v>23</v>
@@ -1488,7 +1446,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" s="4" t="s">
         <v>12</v>
@@ -1511,7 +1469,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19"/>
       <c r="B7" s="8" t="s">
         <v>13</v>
@@ -1529,7 +1487,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="24" t="s">
         <v>16</v>
       </c>
@@ -1539,7 +1497,9 @@
       <c r="C8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="E8" s="10" t="s">
         <v>30</v>
       </c>
@@ -1553,7 +1513,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
       <c r="B9" s="4" t="s">
         <v>45</v>
@@ -1577,7 +1537,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="4" t="s">
         <v>17</v>
@@ -1601,7 +1561,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="4" t="s">
         <v>18</v>
@@ -1625,7 +1585,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="4" t="s">
         <v>19</v>
@@ -1649,7 +1609,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="4" t="s">
         <v>21</v>
@@ -1673,7 +1633,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19"/>
       <c r="B14" s="8" t="s">
         <v>22</v>
@@ -1697,7 +1657,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>24</v>
       </c>
@@ -1721,7 +1681,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="20"/>
       <c r="B16" s="4" t="s">
         <v>31</v>
@@ -1743,7 +1703,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="20"/>
       <c r="B17" s="4" t="s">
         <v>27</v>
@@ -1767,7 +1727,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="20"/>
       <c r="B18" s="4" t="s">
         <v>26</v>
@@ -1789,7 +1749,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="20"/>
       <c r="B19" s="4" t="s">
         <v>28</v>
@@ -1807,7 +1767,7 @@
         <v>43595</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="20"/>
       <c r="B20" s="4" t="s">
         <v>29</v>
@@ -1832,18 +1792,18 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>55</v>
       </c>
       <c r="B23" s="17"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -1855,84 +1815,84 @@
     <mergeCell ref="A15:A20"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="cellIs" dxfId="23" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="47" operator="equal">
       <formula>"EP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="cellIs" dxfId="22" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="46" operator="equal">
       <formula>"U"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="cellIs" dxfId="21" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="45" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:F20">
-    <cfRule type="containsText" dxfId="20" priority="41" operator="containsText" text="pm">
+    <cfRule type="containsText" dxfId="14" priority="41" operator="containsText" text="pm">
       <formula>NOT(ISERROR(SEARCH("pm",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="42" operator="containsText" text="u">
+    <cfRule type="containsText" dxfId="13" priority="42" operator="containsText" text="u">
       <formula>NOT(ISERROR(SEARCH("u",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="43" operator="containsText" text="f">
+    <cfRule type="containsText" dxfId="12" priority="43" operator="containsText" text="f">
       <formula>NOT(ISERROR(SEARCH("f",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="44" operator="containsText" text="ep">
+    <cfRule type="containsText" dxfId="11" priority="44" operator="containsText" text="ep">
       <formula>NOT(ISERROR(SEARCH("ep",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="cellIs" dxfId="16" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="40" operator="equal">
       <formula>"EP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="cellIs" dxfId="15" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="39" operator="equal">
       <formula>"U"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="cellIs" dxfId="14" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="38" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="13" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="33" operator="equal">
       <formula>"EP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="12" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="32" operator="equal">
       <formula>"U"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="11" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="31" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="10" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="26" operator="equal">
       <formula>"EP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="9" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="25" operator="equal">
       <formula>"U"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="8" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="24" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:F20">
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="nt">
+    <cfRule type="containsText" dxfId="1" priority="11" operator="containsText" text="nt">
       <formula>NOT(ISERROR(SEARCH("nt",C2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
       <formula>"nt"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1949,9 +1909,9 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="9" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F9" s="25" t="s">
         <v>4</v>
       </c>
@@ -1968,7 +1928,7 @@
       <c r="Q9" s="26"/>
       <c r="R9" s="26"/>
     </row>
-    <row r="10" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
@@ -1983,7 +1943,7 @@
       <c r="Q10" s="26"/>
       <c r="R10" s="26"/>
     </row>
-    <row r="11" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
@@ -1998,7 +1958,7 @@
       <c r="Q11" s="26"/>
       <c r="R11" s="26"/>
     </row>
-    <row r="12" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
@@ -2013,7 +1973,7 @@
       <c r="Q12" s="26"/>
       <c r="R12" s="26"/>
     </row>
-    <row r="13" spans="6:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>

</xml_diff>